<commit_message>
Update: Configure model for consistency
</commit_message>
<xml_diff>
--- a/output/account_summary_extracted.xlsx
+++ b/output/account_summary_extracted.xlsx
@@ -531,7 +531,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>01-Jan-2024 to 31-Mar-2024</t>
+          <t>01-01-2024 to 31-03-2024</t>
         </is>
       </c>
       <c r="K2" t="inlineStr"/>
@@ -585,7 +585,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>01-Jan-2024</t>
+          <t>01-01-2024</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -612,7 +612,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>03-Jan-2024</t>
+          <t>03-01-2024</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -639,7 +639,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>10-Jan-2024</t>
+          <t>10-01-2024</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -666,7 +666,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>15-Jan-2024</t>
+          <t>15-01-2024</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -689,7 +689,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20-Jan-2024</t>
+          <t>20-01-2024</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -712,7 +712,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>28-Jan-2024</t>
+          <t>28-01-2024</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -735,7 +735,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>03-Feb-2024</t>
+          <t>03-02-2024</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -762,7 +762,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>12-Feb-2024</t>
+          <t>12-02-2024</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -789,7 +789,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>25-Feb-2024</t>
+          <t>25-02-2024</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -816,7 +816,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>01-Mar-2024</t>
+          <t>01-03-2024</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -839,7 +839,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>15-Mar-2024</t>
+          <t>15-03-2024</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -862,7 +862,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>31-Mar-2024</t>
+          <t>31-03-2024</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">

</xml_diff>